<commit_message>
estudo da funcao contse e contses
</commit_message>
<xml_diff>
--- a/Fórmulas e Funções Avançadas/2 - Funções condicionais (SE)/Funções_Condicionais.xlsx
+++ b/Fórmulas e Funções Avançadas/2 - Funções condicionais (SE)/Funções_Condicionais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicam\Desktop\Analista de Dados\Excel\estudos_excel\Fórmulas e Funções Avançadas\2 - Funções condicionais (SE)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B111F154-26CF-430B-A055-26624258C2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B666DDDB-A836-4151-8964-3BDA5C6263DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B3655E84-69E5-4E3D-B55F-C5BC0506C15D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B3655E84-69E5-4E3D-B55F-C5BC0506C15D}"/>
   </bookViews>
   <sheets>
     <sheet name="SE " sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="106">
   <si>
     <t>ID</t>
   </si>
@@ -353,6 +353,21 @@
   </si>
   <si>
     <t>Pagamento Tradicional</t>
+  </si>
+  <si>
+    <t>Incidências =</t>
+  </si>
+  <si>
+    <t>CONT.SE: Serve para contar a quantidade de incidências de determinado critério em uma coluna.</t>
+  </si>
+  <si>
+    <t>CONT.SES: Serve para contar a quantidade de incidências de determinado critério com base em várias colunas</t>
+  </si>
+  <si>
+    <t>Incidência de Venda por Sexo</t>
+  </si>
+  <si>
+    <t>Incidência de Venda por Sexo em Determinado Estado</t>
   </si>
 </sst>
 </file>
@@ -364,7 +379,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,8 +429,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,6 +514,42 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF9966FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF99FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -637,7 +702,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -774,6 +839,41 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1037,6 +1137,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF99FF"/>
       <color rgb="FF9966FF"/>
       <color rgb="FF003399"/>
       <color rgb="FF0DC1C5"/>
@@ -1046,7 +1147,6 @@
       <color rgb="FF47EFF3"/>
       <color rgb="FFFFB3D9"/>
       <color rgb="FFFF3399"/>
-      <color rgb="FFFFD5EA"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1388,7 +1488,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -1478,7 +1578,7 @@
         <v>18</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:H35" si="0">PRODUCT(D3,E3)</f>
+        <f t="shared" ref="G3:G35" si="0">PRODUCT(D3,E3)</f>
         <v>408.24</v>
       </c>
       <c r="H3" s="7" t="str">
@@ -2609,10 +2709,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA469472-C9E1-4B24-B703-537C72B595CD}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:U35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2626,9 +2726,13 @@
     <col min="7" max="7" width="22.42578125" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -2655,7 +2759,7 @@
       </c>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -2680,9 +2784,21 @@
       <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="61" t="s">
+        <v>102</v>
+      </c>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="61"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
+      <c r="U2" s="63"/>
+    </row>
+    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -2707,9 +2823,14 @@
       <c r="H3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+      <c r="O3" s="54"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -2735,8 +2856,13 @@
         <v>19</v>
       </c>
       <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M4" s="55"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="60" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -2762,7 +2888,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -2787,8 +2913,18 @@
       <c r="H6" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N6" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="O6" s="59">
+        <f>COUNTIF(E:E, P6)</f>
+        <v>12</v>
+      </c>
+      <c r="P6" s="67" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -2813,8 +2949,10 @@
       <c r="H7" s="11" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -2840,7 +2978,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -2865,8 +3003,20 @@
       <c r="H9" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="62" t="s">
+        <v>103</v>
+      </c>
+      <c r="L9" s="62"/>
+      <c r="M9" s="62"/>
+      <c r="N9" s="62"/>
+      <c r="O9" s="62"/>
+      <c r="P9" s="62"/>
+      <c r="Q9" s="62"/>
+      <c r="R9" s="62"/>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -2892,7 +3042,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -2917,8 +3067,13 @@
       <c r="H11" s="11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N11" s="64" t="s">
+        <v>105</v>
+      </c>
+      <c r="O11" s="64"/>
+      <c r="P11" s="64"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -2944,7 +3099,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -2969,8 +3124,18 @@
       <c r="H13" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N13" s="65" t="s">
+        <v>101</v>
+      </c>
+      <c r="O13" s="44">
+        <f>COUNTIFS(E:E, P13, H:H, P14)</f>
+        <v>9</v>
+      </c>
+      <c r="P13" s="66" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -2995,8 +3160,11 @@
       <c r="H14" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="P14" s="68" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -3022,7 +3190,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -3544,6 +3712,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:H35" xr:uid="{FA469472-C9E1-4B24-B703-537C72B595CD}"/>
+  <mergeCells count="3">
+    <mergeCell ref="K9:T9"/>
+    <mergeCell ref="K2:T2"/>
+    <mergeCell ref="N11:P11"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
estudo pratico de procv
</commit_message>
<xml_diff>
--- a/Fórmulas e Funções Avançadas/2 - Funções condicionais (SE)/Funções_Condicionais.xlsx
+++ b/Fórmulas e Funções Avançadas/2 - Funções condicionais (SE)/Funções_Condicionais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicam\Desktop\Analista de Dados\Excel\estudos_excel\Fórmulas e Funções Avançadas\2 - Funções condicionais (SE)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394FA180-F00C-49F8-9CAE-F8B4958AAA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCC4E07-7019-490E-820B-EEF8941355E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B3655E84-69E5-4E3D-B55F-C5BC0506C15D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B3655E84-69E5-4E3D-B55F-C5BC0506C15D}"/>
   </bookViews>
   <sheets>
     <sheet name="SE " sheetId="2" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="116">
   <si>
     <t>ID</t>
   </si>
@@ -358,12 +358,6 @@
     <t>Incidências =</t>
   </si>
   <si>
-    <t>CONT.SE: Serve para contar a quantidade de incidências de determinado critério em uma coluna.</t>
-  </si>
-  <si>
-    <t>CONT.SES: Serve para contar a quantidade de incidências de determinado critério com base em várias colunas</t>
-  </si>
-  <si>
     <t>Incidência de Venda por Sexo</t>
   </si>
   <si>
@@ -373,10 +367,137 @@
     <t>Incidência de Venda do Estado</t>
   </si>
   <si>
-    <t>SOMASE: Serve para somar valores com base na quantidade de incidências de outro critério estabelecido.</t>
-  </si>
-  <si>
-    <t>SOMASES:  Serve para somar valores com base na quantidade de incidências de outros critérios estabelecido.</t>
+    <t>e</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SOMASE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Serve para somar valores com base na quantidade de incidências de outro critério estabelecido.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SOMASES:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  Serve para somar valores com base na quantidade de incidências de outros critérios estabelecido.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CONT.SE:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Serve para contar a quantidade de incidências de determinado critério em uma coluna.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CONT.SES:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Serve para contar a quantidade de incidências de determinado critério com base em várias colunas</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PROCV:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> é usada para buscar um valor em uma coluna de uma tabela e retornar um valor correspondente de outra coluna na mesma linha.</t>
+    </r>
+  </si>
+  <si>
+    <t>*Para ver a tabela de gerentes é necessário reexibí-las.</t>
+  </si>
+  <si>
+    <t>Nesse caso, buscou-se os gerentes, na tabela oculta "Base de Gerentes", utilizando a coluna "Loja" como referência.</t>
+  </si>
+  <si>
+    <t>a primeira coluna dessa tabela seja igual ao valor_procurado na fórmula do PROCV.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ao selecionar uma tabela para ser utilizada como base para a tabela a ser aplicada o PROCV, é necessário que </t>
+  </si>
+  <si>
+    <t>Além disso, o núm_índice_coluna da fórmula se trata da coluna (A, B, C...) contada em números (A = 1, B = 2...).</t>
   </si>
 </sst>
 </file>
@@ -388,7 +509,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -452,8 +573,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="19">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -559,6 +688,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,7 +864,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -865,6 +1018,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -877,17 +1042,23 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1152,6 +1323,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FFFF9966"/>
       <color rgb="FFFF99FF"/>
       <color rgb="FF9966FF"/>
       <color rgb="FF003399"/>
@@ -1160,8 +1333,6 @@
       <color rgb="FF10E9EE"/>
       <color rgb="FF18EBF0"/>
       <color rgb="FF47EFF3"/>
-      <color rgb="FFFFB3D9"/>
-      <color rgb="FFFF3399"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2727,7 +2898,7 @@
   <dimension ref="A1:U35"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T14" sqref="K2:T14"/>
+      <selection activeCell="K9" sqref="K9:T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2799,18 +2970,18 @@
       <c r="H2" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62"/>
-      <c r="N2" s="62"/>
-      <c r="O2" s="62"/>
-      <c r="P2" s="62"/>
-      <c r="Q2" s="62"/>
-      <c r="R2" s="62"/>
-      <c r="S2" s="62"/>
-      <c r="T2" s="62"/>
+      <c r="K2" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="L2" s="66"/>
+      <c r="M2" s="66"/>
+      <c r="N2" s="66"/>
+      <c r="O2" s="66"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="66"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="66"/>
+      <c r="T2" s="66"/>
       <c r="U2" s="57"/>
     </row>
     <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2873,7 +3044,7 @@
       <c r="J4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="56" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -3015,18 +3186,18 @@
       <c r="H9" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="61" t="s">
-        <v>103</v>
-      </c>
-      <c r="L9" s="61"/>
-      <c r="M9" s="61"/>
-      <c r="N9" s="61"/>
-      <c r="O9" s="61"/>
-      <c r="P9" s="61"/>
-      <c r="Q9" s="61"/>
-      <c r="R9" s="61"/>
-      <c r="S9" s="61"/>
-      <c r="T9" s="61"/>
+      <c r="K9" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="L9" s="65"/>
+      <c r="M9" s="65"/>
+      <c r="N9" s="65"/>
+      <c r="O9" s="65"/>
+      <c r="P9" s="65"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="65"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="65"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
@@ -3079,11 +3250,11 @@
       <c r="H11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="63" t="s">
-        <v>105</v>
-      </c>
-      <c r="O11" s="63"/>
-      <c r="P11" s="63"/>
+      <c r="N11" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="O11" s="67"/>
+      <c r="P11" s="67"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
@@ -3737,8 +3908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B00C4A2D-A2CC-45A5-89A7-8AF9B7C6F3FC}">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13:V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3815,7 +3986,7 @@
       <c r="I2" s="16">
         <v>303.52</v>
       </c>
-      <c r="K2" s="66"/>
+      <c r="K2" s="62"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="14">
@@ -3934,20 +4105,20 @@
       <c r="I6" s="16">
         <v>92.8</v>
       </c>
-      <c r="K6" s="62" t="s">
-        <v>107</v>
-      </c>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62"/>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="62"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="62"/>
-      <c r="T6" s="62"/>
-      <c r="U6" s="62"/>
-      <c r="V6" s="62"/>
+      <c r="K6" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="66"/>
+      <c r="S6" s="66"/>
+      <c r="T6" s="66"/>
+      <c r="U6" s="66"/>
+      <c r="V6" s="66"/>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
@@ -4011,11 +4182,11 @@
       <c r="I8" s="16">
         <v>66.25</v>
       </c>
-      <c r="N8" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="O8" s="64"/>
-      <c r="P8" s="64"/>
+      <c r="N8" s="68" t="s">
+        <v>104</v>
+      </c>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
@@ -4077,7 +4248,7 @@
       <c r="N10" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="O10" s="65">
+      <c r="O10" s="61">
         <f>SUMIF(H:H,P10, I:I)</f>
         <v>10720.529999999999</v>
       </c>
@@ -4171,20 +4342,20 @@
       <c r="I13" s="16">
         <v>285.78000000000003</v>
       </c>
-      <c r="K13" s="61" t="s">
-        <v>108</v>
-      </c>
-      <c r="L13" s="61"/>
-      <c r="M13" s="61"/>
-      <c r="N13" s="61"/>
-      <c r="O13" s="61"/>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="61"/>
-      <c r="S13" s="61"/>
-      <c r="T13" s="61"/>
-      <c r="U13" s="61"/>
-      <c r="V13" s="61"/>
+      <c r="K13" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+      <c r="N13" s="65"/>
+      <c r="O13" s="65"/>
+      <c r="P13" s="65"/>
+      <c r="Q13" s="65"/>
+      <c r="R13" s="65"/>
+      <c r="S13" s="65"/>
+      <c r="T13" s="65"/>
+      <c r="U13" s="65"/>
+      <c r="V13" s="65"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="14">
@@ -4243,13 +4414,13 @@
       <c r="I15" s="16">
         <v>278.39999999999998</v>
       </c>
-      <c r="N15" s="63" t="s">
-        <v>105</v>
-      </c>
-      <c r="O15" s="63"/>
-      <c r="P15" s="63"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="63"/>
+      <c r="N15" s="67" t="s">
+        <v>103</v>
+      </c>
+      <c r="O15" s="67"/>
+      <c r="P15" s="67"/>
+      <c r="Q15" s="67"/>
+      <c r="R15" s="67"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="14">
@@ -4311,7 +4482,7 @@
       <c r="N17" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="O17" s="68">
+      <c r="O17" s="64">
         <f>SUMIFS(I:I,H:H,P17,G:G,P18)</f>
         <v>1190.2299999999998</v>
       </c>
@@ -4347,7 +4518,7 @@
       <c r="I18" s="16">
         <v>2227.17</v>
       </c>
-      <c r="P18" s="67" t="s">
+      <c r="P18" s="63" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4858,9 +5029,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3E3B50-FFAA-4324-8586-2D81EE6BC0CC}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4875,7 +5048,7 @@
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
@@ -4900,9 +5073,19 @@
       <c r="I1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="21"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J1" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="70" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
         <v>11</v>
       </c>
@@ -4928,9 +5111,12 @@
       <c r="I2" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="J2" s="29"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J2" s="29" t="str">
+        <f>VLOOKUP(J1,Tabela5[#All],7,)</f>
+        <v>Julia Ramos</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
         <v>42</v>
       </c>
@@ -4954,7 +5140,7 @@
         <v>Carmem Silva</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
         <v>32</v>
       </c>
@@ -4978,7 +5164,7 @@
         <v>Gabriel Gomes</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
         <v>60</v>
       </c>
@@ -5001,8 +5187,22 @@
         <f>VLOOKUP(F5,'Base de Gerentes'!A:B,2,)</f>
         <v>Carmem Silva</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="69" t="s">
+        <v>110</v>
+      </c>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
         <v>72</v>
       </c>
@@ -5026,7 +5226,7 @@
         <v>Carmem Silva</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>75</v>
       </c>
@@ -5049,8 +5249,21 @@
         <f>VLOOKUP(F7,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I7" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="71"/>
+      <c r="O7" s="71"/>
+      <c r="P7" s="71"/>
+      <c r="Q7" s="71"/>
+      <c r="R7" s="71"/>
+      <c r="S7" s="71"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
         <v>59</v>
       </c>
@@ -5074,7 +5287,7 @@
         <v>Julia Ramos</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>70</v>
       </c>
@@ -5097,8 +5310,21 @@
         <f>VLOOKUP(F9,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I9" s="73" t="s">
+        <v>114</v>
+      </c>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="72"/>
+      <c r="Q9" s="72"/>
+      <c r="R9" s="72"/>
+      <c r="S9" s="72"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>21</v>
       </c>
@@ -5121,8 +5347,18 @@
         <f>VLOOKUP(F10,'Base de Gerentes'!A:B,2,)</f>
         <v>Julia Ramos</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J10" s="73" t="s">
+        <v>113</v>
+      </c>
+      <c r="K10" s="73"/>
+      <c r="L10" s="73"/>
+      <c r="M10" s="73"/>
+      <c r="N10" s="73"/>
+      <c r="O10" s="73"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="73"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
         <v>36</v>
       </c>
@@ -5146,7 +5382,7 @@
         <v>Gabriel Gomes</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>51</v>
       </c>
@@ -5169,8 +5405,21 @@
         <f>VLOOKUP(F12,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I12" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="J12" s="74"/>
+      <c r="K12" s="74"/>
+      <c r="L12" s="74"/>
+      <c r="M12" s="74"/>
+      <c r="N12" s="74"/>
+      <c r="O12" s="74"/>
+      <c r="P12" s="74"/>
+      <c r="Q12" s="74"/>
+      <c r="R12" s="74"/>
+      <c r="S12" s="74"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>49</v>
       </c>
@@ -5194,7 +5443,7 @@
         <v>Roberto Lopes</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="20" t="s">
         <v>77</v>
       </c>
@@ -5218,7 +5467,7 @@
         <v>Julia Ramos</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
         <v>74</v>
       </c>
@@ -5242,7 +5491,7 @@
         <v>Julia Ramos</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>30</v>
       </c>
@@ -5795,6 +6044,14 @@
       <c r="G43"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="I5:T5"/>
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="I9:S9"/>
+    <mergeCell ref="J10:Q10"/>
+    <mergeCell ref="I12:S12"/>
+    <mergeCell ref="I7:S7"/>
+  </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B35" xr:uid="{F9E1B015-2713-4476-9881-9BB5E81FBE5A}">
@@ -7425,7 +7682,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
estudo pratico de proch e procx
</commit_message>
<xml_diff>
--- a/Fórmulas e Funções Avançadas/2 - Funções condicionais (SE)/Funções_Condicionais.xlsx
+++ b/Fórmulas e Funções Avançadas/2 - Funções condicionais (SE)/Funções_Condicionais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicam\Desktop\Analista de Dados\Excel\estudos_excel\Fórmulas e Funções Avançadas\2 - Funções condicionais (SE)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCC4E07-7019-490E-820B-EEF8941355E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74A7FE9-A3EB-409A-9B40-A50ADAE5C097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B3655E84-69E5-4E3D-B55F-C5BC0506C15D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{B3655E84-69E5-4E3D-B55F-C5BC0506C15D}"/>
   </bookViews>
   <sheets>
     <sheet name="SE " sheetId="2" r:id="rId1"/>
@@ -20,12 +20,12 @@
     <sheet name="PROCH" sheetId="10" r:id="rId5"/>
     <sheet name="Base de Gerentes" sheetId="8" state="hidden" r:id="rId6"/>
     <sheet name="PROCX" sheetId="7" r:id="rId7"/>
-    <sheet name="Base de Vendedores" sheetId="9" state="hidden" r:id="rId8"/>
+    <sheet name="Base de Vendedores" sheetId="9" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CONT.SE e CONT.SES'!$A$1:$H$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PROCV!#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">PROCX!$A$1:$L$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">PROCX!$A$1:$M$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SE '!$A$1:$H$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'SOMASE e SOMASES'!$A$1:$I$35</definedName>
   </definedNames>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="117">
   <si>
     <t>ID</t>
   </si>
@@ -365,9 +365,6 @@
   </si>
   <si>
     <t>Incidência de Venda do Estado</t>
-  </si>
-  <si>
-    <t>e</t>
   </si>
   <si>
     <r>
@@ -498,6 +495,32 @@
   </si>
   <si>
     <t>Além disso, o núm_índice_coluna da fórmula se trata da coluna (A, B, C...) contada em números (A = 1, B = 2...).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">PROCH: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Funciona da mesma forma que o PROCV, mas dessa vez busca o valor em uma linha da tabela ao invés de uma coluna. </t>
+    </r>
+  </si>
+  <si>
+    <t>Código do Vendedor</t>
   </si>
 </sst>
 </file>
@@ -716,7 +739,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -859,12 +882,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF0DC1C5"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1048,17 +1080,20 @@
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2971,7 +3006,7 @@
         <v>14</v>
       </c>
       <c r="K2" s="66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="L2" s="66"/>
       <c r="M2" s="66"/>
@@ -3187,7 +3222,7 @@
         <v>28</v>
       </c>
       <c r="K9" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="L9" s="65"/>
       <c r="M9" s="65"/>
@@ -4106,7 +4141,7 @@
         <v>92.8</v>
       </c>
       <c r="K6" s="66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L6" s="66"/>
       <c r="M6" s="66"/>
@@ -4343,7 +4378,7 @@
         <v>285.78000000000003</v>
       </c>
       <c r="K13" s="65" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="L13" s="65"/>
       <c r="M13" s="65"/>
@@ -5031,8 +5066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E3E3B50-FFAA-4324-8586-2D81EE6BC0CC}">
   <dimension ref="A1:T43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5077,7 +5112,7 @@
         <v>16</v>
       </c>
       <c r="L1" s="70" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M1" s="70"/>
       <c r="N1" s="70"/>
@@ -5188,7 +5223,7 @@
         <v>Carmem Silva</v>
       </c>
       <c r="I5" s="69" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J5" s="69"/>
       <c r="K5" s="69"/>
@@ -5249,19 +5284,19 @@
         <f>VLOOKUP(F7,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="I7" s="71" t="s">
-        <v>112</v>
-      </c>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
-      <c r="O7" s="71"/>
-      <c r="P7" s="71"/>
-      <c r="Q7" s="71"/>
-      <c r="R7" s="71"/>
-      <c r="S7" s="71"/>
+      <c r="I7" s="74" t="s">
+        <v>111</v>
+      </c>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
@@ -5310,8 +5345,8 @@
         <f>VLOOKUP(F9,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="I9" s="73" t="s">
-        <v>114</v>
+      <c r="I9" s="71" t="s">
+        <v>113</v>
       </c>
       <c r="J9" s="72"/>
       <c r="K9" s="72"/>
@@ -5347,16 +5382,16 @@
         <f>VLOOKUP(F10,'Base de Gerentes'!A:B,2,)</f>
         <v>Julia Ramos</v>
       </c>
-      <c r="J10" s="73" t="s">
-        <v>113</v>
-      </c>
-      <c r="K10" s="73"/>
-      <c r="L10" s="73"/>
-      <c r="M10" s="73"/>
-      <c r="N10" s="73"/>
-      <c r="O10" s="73"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="73"/>
+      <c r="J10" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
+      <c r="N10" s="71"/>
+      <c r="O10" s="71"/>
+      <c r="P10" s="71"/>
+      <c r="Q10" s="71"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
@@ -5405,19 +5440,19 @@
         <f>VLOOKUP(F12,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="I12" s="74" t="s">
-        <v>115</v>
-      </c>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
-      <c r="M12" s="74"/>
-      <c r="N12" s="74"/>
-      <c r="O12" s="74"/>
-      <c r="P12" s="74"/>
-      <c r="Q12" s="74"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="74"/>
+      <c r="I12" s="73" t="s">
+        <v>114</v>
+      </c>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="73"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="73"/>
+      <c r="R12" s="73"/>
+      <c r="S12" s="73"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
@@ -6067,9 +6102,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505EA35A-C318-414B-9391-6442CB704F91}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6082,7 +6119,7 @@
     <col min="7" max="7" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>79</v>
       </c>
@@ -6099,7 +6136,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>8</v>
       </c>
@@ -6115,8 +6152,11 @@
       <c r="E2" s="40" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="75" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>92</v>
       </c>
@@ -6133,7 +6173,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="42" t="s">
         <v>97</v>
       </c>
@@ -6150,7 +6190,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="42" t="s">
         <v>98</v>
       </c>
@@ -6167,7 +6207,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="42" t="s">
         <v>9</v>
       </c>
@@ -6184,7 +6224,7 @@
         <v>7959.64</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="39" t="s">
         <v>79</v>
       </c>
@@ -6192,7 +6232,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="42" t="s">
         <v>97</v>
       </c>
@@ -6274,9 +6314,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF5F63A-A48A-466D-9D12-E052B07C29AE}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6285,16 +6327,17 @@
     <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" style="3" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
-    <col min="11" max="11" width="23.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
@@ -6311,28 +6354,31 @@
         <v>4</v>
       </c>
       <c r="F1" s="46" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="H1" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="I1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="J1" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="K1" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="46" t="s">
+      <c r="L1" s="46" t="s">
         <v>78</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="M1" s="48" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="49">
         <v>1</v>
       </c>
@@ -6348,30 +6394,34 @@
       <c r="E2" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E2,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>ANDEFE001</v>
+      </c>
+      <c r="G2" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="49">
+      <c r="H2" s="49">
         <v>7</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="I2" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="51" t="str">
-        <f>VLOOKUP(H2,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J2" s="51" t="str">
+        <f>VLOOKUP(I2,'Base de Gerentes'!A:B,2,)</f>
         <v>Carmem Silva</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="K2" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="L2" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="L2" s="52">
+      <c r="M2" s="52">
         <v>303.52</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="49">
         <v>2</v>
       </c>
@@ -6387,30 +6437,34 @@
       <c r="E3" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="49">
+      <c r="F3" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E3,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>ISERMA0018</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="49">
         <v>9</v>
       </c>
-      <c r="H3" s="51" t="s">
+      <c r="I3" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="51" t="str">
-        <f>VLOOKUP(H3,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J3" s="51" t="str">
+        <f>VLOOKUP(I3,'Base de Gerentes'!A:B,2,)</f>
         <v>Julia Ramos</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="K3" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="51" t="s">
+      <c r="L3" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L3" s="52">
+      <c r="M3" s="52">
         <v>408.24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="49">
         <v>3</v>
       </c>
@@ -6426,30 +6480,34 @@
       <c r="E4" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E4,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>CEESFE009</v>
+      </c>
+      <c r="G4" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="49">
+      <c r="H4" s="49">
         <v>5</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="I4" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="51" t="str">
-        <f>VLOOKUP(H4,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J4" s="51" t="str">
+        <f>VLOOKUP(I4,'Base de Gerentes'!A:B,2,)</f>
         <v>Julia Ramos</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="K4" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="51" t="s">
+      <c r="L4" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="L4" s="52">
+      <c r="M4" s="52">
         <v>62.599999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="49">
         <v>4</v>
       </c>
@@ -6465,30 +6523,34 @@
       <c r="E5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="49">
+      <c r="F5" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E5,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>YUERMA0032</v>
+      </c>
+      <c r="G5" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="49">
         <v>7</v>
       </c>
-      <c r="H5" s="51" t="s">
+      <c r="I5" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="51" t="str">
-        <f>VLOOKUP(H5,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J5" s="51" t="str">
+        <f>VLOOKUP(I5,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J5" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K5" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L5" s="52">
+      <c r="M5" s="52">
         <v>181.09</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="49">
         <v>5</v>
       </c>
@@ -6504,30 +6566,34 @@
       <c r="E6" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="51" t="s">
+      <c r="F6" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E6,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>PIESFE0026</v>
+      </c>
+      <c r="G6" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="49">
+      <c r="H6" s="49">
         <v>5</v>
       </c>
-      <c r="H6" s="51" t="s">
+      <c r="I6" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="51" t="str">
-        <f>VLOOKUP(H6,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J6" s="51" t="str">
+        <f>VLOOKUP(I6,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="J6" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K6" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L6" s="52">
+      <c r="M6" s="52">
         <v>92.8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="49">
         <v>6</v>
       </c>
@@ -6543,30 +6609,34 @@
       <c r="E7" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="F7" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E7,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>FEESFE0015</v>
+      </c>
+      <c r="G7" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="49">
+      <c r="H7" s="49">
         <v>7</v>
       </c>
-      <c r="H7" s="51" t="s">
+      <c r="I7" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="51" t="str">
-        <f>VLOOKUP(H7,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J7" s="51" t="str">
+        <f>VLOOKUP(I7,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J7" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K7" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L7" s="52">
+      <c r="M7" s="52">
         <v>1417.29</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="49">
         <v>7</v>
       </c>
@@ -6582,30 +6652,34 @@
       <c r="E8" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="49">
+      <c r="F8" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E8,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>ANESMA003</v>
+      </c>
+      <c r="G8" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="49">
         <v>5</v>
       </c>
-      <c r="H8" s="51" t="s">
+      <c r="I8" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="51" t="str">
-        <f>VLOOKUP(H8,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J8" s="51" t="str">
+        <f>VLOOKUP(I8,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="J8" s="51" t="s">
+      <c r="K8" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="51" t="s">
+      <c r="L8" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L8" s="52">
+      <c r="M8" s="52">
         <v>66.25</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="49">
         <v>8</v>
       </c>
@@ -6621,30 +6695,34 @@
       <c r="E9" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E9,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>VIRAFE0030</v>
+      </c>
+      <c r="G9" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="49">
+      <c r="H9" s="49">
         <v>8</v>
       </c>
-      <c r="H9" s="51" t="s">
+      <c r="I9" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="51" t="str">
-        <f>VLOOKUP(H9,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J9" s="51" t="str">
+        <f>VLOOKUP(I9,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="J9" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K9" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L9" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="52">
+      <c r="M9" s="52">
         <v>151.68</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="49">
         <v>9</v>
       </c>
@@ -6660,30 +6738,34 @@
       <c r="E10" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="49">
+      <c r="F10" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E10,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>DATOMA0010</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="49">
         <v>14</v>
       </c>
-      <c r="H10" s="51" t="s">
+      <c r="I10" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="51" t="str">
-        <f>VLOOKUP(H10,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J10" s="51" t="str">
+        <f>VLOOKUP(I10,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="J10" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K10" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L10" s="52">
+      <c r="M10" s="52">
         <v>251.72</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="49">
         <v>10</v>
       </c>
@@ -6699,30 +6781,34 @@
       <c r="E11" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E11,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>MAHOFE0023</v>
+      </c>
+      <c r="G11" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="49">
+      <c r="H11" s="49">
         <v>5</v>
       </c>
-      <c r="H11" s="51" t="s">
+      <c r="I11" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="51" t="str">
-        <f>VLOOKUP(H11,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J11" s="51" t="str">
+        <f>VLOOKUP(I11,'Base de Gerentes'!A:B,2,)</f>
         <v>Julia Ramos</v>
       </c>
-      <c r="J11" s="51" t="s">
+      <c r="K11" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="51" t="s">
+      <c r="L11" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L11" s="52">
+      <c r="M11" s="52">
         <v>94.9</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="49">
         <v>11</v>
       </c>
@@ -6738,30 +6824,34 @@
       <c r="E12" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="49">
+      <c r="F12" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E12,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>PITOMA0028</v>
+      </c>
+      <c r="G12" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="49">
         <v>14</v>
       </c>
-      <c r="H12" s="51" t="s">
+      <c r="I12" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="51" t="str">
-        <f>VLOOKUP(H12,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J12" s="51" t="str">
+        <f>VLOOKUP(I12,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J12" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K12" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L12" s="52">
+      <c r="M12" s="52">
         <v>193.9</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="49">
         <v>12</v>
       </c>
@@ -6777,30 +6867,34 @@
       <c r="E13" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="51" t="s">
+      <c r="F13" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E13,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>ANHAFE002</v>
+      </c>
+      <c r="G13" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="49">
+      <c r="H13" s="49">
         <v>11</v>
       </c>
-      <c r="H13" s="51" t="s">
+      <c r="I13" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="51" t="str">
-        <f>VLOOKUP(H13,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J13" s="51" t="str">
+        <f>VLOOKUP(I13,'Base de Gerentes'!A:B,2,)</f>
         <v>Carmem Silva</v>
       </c>
-      <c r="J13" s="51" t="s">
+      <c r="K13" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K13" s="51" t="s">
+      <c r="L13" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="L13" s="52">
+      <c r="M13" s="52">
         <v>285.78000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="49">
         <v>13</v>
       </c>
@@ -6816,30 +6910,34 @@
       <c r="E14" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="51" t="s">
+      <c r="F14" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E14,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>VIRAFE0030</v>
+      </c>
+      <c r="G14" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="49">
+      <c r="H14" s="49">
         <v>9</v>
       </c>
-      <c r="H14" s="51" t="s">
+      <c r="I14" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="51" t="str">
-        <f>VLOOKUP(H14,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J14" s="51" t="str">
+        <f>VLOOKUP(I14,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="J14" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K14" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L14" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L14" s="52">
+      <c r="M14" s="52">
         <v>170.82</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="49">
         <v>14</v>
       </c>
@@ -6855,30 +6953,34 @@
       <c r="E15" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="F15" s="51" t="s">
+      <c r="F15" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E15,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>LUIOFE0022</v>
+      </c>
+      <c r="G15" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="49">
+      <c r="H15" s="49">
         <v>15</v>
       </c>
-      <c r="H15" s="51" t="s">
+      <c r="I15" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="51" t="str">
-        <f>VLOOKUP(H15,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J15" s="51" t="str">
+        <f>VLOOKUP(I15,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J15" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K15" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L15" s="52">
+      <c r="M15" s="52">
         <v>278.39999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="49">
         <v>15</v>
       </c>
@@ -6894,30 +6996,34 @@
       <c r="E16" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="49">
+      <c r="F16" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E16,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>PETAMA0025</v>
+      </c>
+      <c r="G16" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="49">
         <v>5</v>
       </c>
-      <c r="H16" s="51" t="s">
+      <c r="I16" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="51" t="str">
-        <f>VLOOKUP(H16,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J16" s="51" t="str">
+        <f>VLOOKUP(I16,'Base de Gerentes'!A:B,2,)</f>
         <v>Carmem Silva</v>
       </c>
-      <c r="J16" s="51" t="s">
+      <c r="K16" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="51" t="s">
+      <c r="L16" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="L16" s="52">
+      <c r="M16" s="52">
         <v>66.8</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="49">
         <v>16</v>
       </c>
@@ -6933,30 +7039,34 @@
       <c r="E17" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G17" s="49">
+      <c r="F17" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E17,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>PETAMA0025</v>
+      </c>
+      <c r="G17" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="49">
         <v>5</v>
       </c>
-      <c r="H17" s="51" t="s">
+      <c r="I17" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="51" t="str">
-        <f>VLOOKUP(H17,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J17" s="51" t="str">
+        <f>VLOOKUP(I17,'Base de Gerentes'!A:B,2,)</f>
         <v>Carmem Silva</v>
       </c>
-      <c r="J17" s="51" t="s">
+      <c r="K17" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K17" s="51" t="s">
+      <c r="L17" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="L17" s="52">
+      <c r="M17" s="52">
         <v>149.9</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="49">
         <v>17</v>
       </c>
@@ -6972,30 +7082,34 @@
       <c r="E18" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G18" s="49">
+      <c r="F18" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E18,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>DAOAMA0012</v>
+      </c>
+      <c r="G18" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="49">
         <v>11</v>
       </c>
-      <c r="H18" s="51" t="s">
+      <c r="I18" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="51" t="str">
-        <f>VLOOKUP(H18,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J18" s="51" t="str">
+        <f>VLOOKUP(I18,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J18" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K18" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L18" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L18" s="52">
+      <c r="M18" s="52">
         <v>2227.17</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="49">
         <v>18</v>
       </c>
@@ -7011,30 +7125,34 @@
       <c r="E19" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="F19" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="49">
+      <c r="F19" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E19,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>DAESMA0011</v>
+      </c>
+      <c r="G19" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="49">
         <v>10</v>
       </c>
-      <c r="H19" s="51" t="s">
+      <c r="I19" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I19" s="51" t="str">
-        <f>VLOOKUP(H19,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J19" s="51" t="str">
+        <f>VLOOKUP(I19,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="J19" s="51" t="s">
+      <c r="K19" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="K19" s="51" t="s">
+      <c r="L19" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L19" s="52">
+      <c r="M19" s="52">
         <v>356.2</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="49">
         <v>19</v>
       </c>
@@ -7050,30 +7168,34 @@
       <c r="E20" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="49">
+      <c r="F20" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E20,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>THRAMA0029</v>
+      </c>
+      <c r="G20" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="49">
         <v>9</v>
       </c>
-      <c r="H20" s="51" t="s">
+      <c r="I20" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="51" t="str">
-        <f>VLOOKUP(H20,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J20" s="51" t="str">
+        <f>VLOOKUP(I20,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J20" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K20" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L20" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L20" s="52">
+      <c r="M20" s="52">
         <v>305.91000000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="49">
         <v>20</v>
       </c>
@@ -7089,30 +7211,34 @@
       <c r="E21" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G21" s="49">
+      <c r="F21" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E21,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>MADEMA0024</v>
+      </c>
+      <c r="G21" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="49">
         <v>15</v>
       </c>
-      <c r="H21" s="51" t="s">
+      <c r="I21" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I21" s="51" t="str">
-        <f>VLOOKUP(H21,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J21" s="51" t="str">
+        <f>VLOOKUP(I21,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J21" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K21" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L21" s="52">
+      <c r="M21" s="52">
         <v>258</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="49">
         <v>21</v>
       </c>
@@ -7128,30 +7254,34 @@
       <c r="E22" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="F22" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="49">
+      <c r="F22" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E22,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>YATAMA0031</v>
+      </c>
+      <c r="G22" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="49">
         <v>14</v>
       </c>
-      <c r="H22" s="51" t="s">
+      <c r="I22" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I22" s="51" t="str">
-        <f>VLOOKUP(H22,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J22" s="51" t="str">
+        <f>VLOOKUP(I22,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="J22" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K22" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L22" s="52">
+      <c r="M22" s="52">
         <v>404.59999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="49">
         <v>22</v>
       </c>
@@ -7167,30 +7297,34 @@
       <c r="E23" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="F23" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G23" s="49">
+      <c r="F23" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E23,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>GAERMA0016</v>
+      </c>
+      <c r="G23" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="49">
         <v>8</v>
       </c>
-      <c r="H23" s="51" t="s">
+      <c r="I23" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="51" t="str">
-        <f>VLOOKUP(H23,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J23" s="51" t="str">
+        <f>VLOOKUP(I23,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J23" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K23" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L23" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L23" s="52">
+      <c r="M23" s="52">
         <v>346.88</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="49">
         <v>23</v>
       </c>
@@ -7206,30 +7340,34 @@
       <c r="E24" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="F24" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="49">
+      <c r="F24" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E24,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>CADOMA007</v>
+      </c>
+      <c r="G24" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="49">
         <v>11</v>
       </c>
-      <c r="H24" s="51" t="s">
+      <c r="I24" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="I24" s="51" t="str">
-        <f>VLOOKUP(H24,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J24" s="51" t="str">
+        <f>VLOOKUP(I24,'Base de Gerentes'!A:B,2,)</f>
         <v>Julia Ramos</v>
       </c>
-      <c r="J24" s="51" t="s">
+      <c r="K24" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="K24" s="51" t="s">
+      <c r="L24" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L24" s="52">
+      <c r="M24" s="52">
         <v>2227.17</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="49">
         <v>24</v>
       </c>
@@ -7245,30 +7383,34 @@
       <c r="E25" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="F25" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="49">
+      <c r="F25" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E25,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>ARESMA004</v>
+      </c>
+      <c r="G25" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="49">
         <v>11</v>
       </c>
-      <c r="H25" s="51" t="s">
+      <c r="I25" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="51" t="str">
-        <f>VLOOKUP(H25,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J25" s="51" t="str">
+        <f>VLOOKUP(I25,'Base de Gerentes'!A:B,2,)</f>
         <v>Carmem Silva</v>
       </c>
-      <c r="J25" s="51" t="s">
+      <c r="K25" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K25" s="51" t="s">
+      <c r="L25" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="L25" s="52">
+      <c r="M25" s="52">
         <v>197.78</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="49">
         <v>25</v>
       </c>
@@ -7284,30 +7426,34 @@
       <c r="E26" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="F26" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="49">
+      <c r="F26" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E26,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>LOELMA0020</v>
+      </c>
+      <c r="G26" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="49">
         <v>11</v>
       </c>
-      <c r="H26" s="51" t="s">
+      <c r="I26" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I26" s="51" t="str">
-        <f>VLOOKUP(H26,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J26" s="51" t="str">
+        <f>VLOOKUP(I26,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J26" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K26" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L26" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L26" s="52">
+      <c r="M26" s="52">
         <v>150.15</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="49">
         <v>26</v>
       </c>
@@ -7323,30 +7469,34 @@
       <c r="E27" s="51" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G27" s="49">
+      <c r="F27" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E27,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>GUÇAMA0017</v>
+      </c>
+      <c r="G27" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="49">
         <v>13</v>
       </c>
-      <c r="H27" s="51" t="s">
+      <c r="I27" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I27" s="51" t="str">
-        <f>VLOOKUP(H27,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J27" s="51" t="str">
+        <f>VLOOKUP(I27,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="J27" s="51" t="s">
+      <c r="K27" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K27" s="51" t="s">
+      <c r="L27" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="L27" s="52">
+      <c r="M27" s="52">
         <v>5958.16</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="49">
         <v>27</v>
       </c>
@@ -7362,30 +7512,34 @@
       <c r="E28" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="F28" s="51" t="s">
+      <c r="F28" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E28,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>LEHAFE0019</v>
+      </c>
+      <c r="G28" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="49">
+      <c r="H28" s="49">
         <v>11</v>
       </c>
-      <c r="H28" s="51" t="s">
+      <c r="I28" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I28" s="51" t="str">
-        <f>VLOOKUP(H28,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J28" s="51" t="str">
+        <f>VLOOKUP(I28,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J28" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K28" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L28" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L28" s="52">
+      <c r="M28" s="52">
         <v>2227.17</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="49">
         <v>28</v>
       </c>
@@ -7401,30 +7555,34 @@
       <c r="E29" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="F29" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="49">
+      <c r="F29" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E29,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>PIESMA0027</v>
+      </c>
+      <c r="G29" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H29" s="49">
         <v>5</v>
       </c>
-      <c r="H29" s="51" t="s">
+      <c r="I29" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I29" s="51" t="str">
-        <f>VLOOKUP(H29,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J29" s="51" t="str">
+        <f>VLOOKUP(I29,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J29" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K29" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L29" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L29" s="52">
+      <c r="M29" s="52">
         <v>69.45</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="49">
         <v>29</v>
       </c>
@@ -7440,30 +7598,34 @@
       <c r="E30" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="49">
+      <c r="F30" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E30,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>LUOSMA0021</v>
+      </c>
+      <c r="G30" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H30" s="49">
         <v>14</v>
       </c>
-      <c r="H30" s="51" t="s">
+      <c r="I30" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I30" s="51" t="str">
-        <f>VLOOKUP(H30,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J30" s="51" t="str">
+        <f>VLOOKUP(I30,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="J30" s="51" t="s">
+      <c r="K30" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="K30" s="51" t="s">
+      <c r="L30" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L30" s="52">
+      <c r="M30" s="52">
         <v>2834.58</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="49">
         <v>30</v>
       </c>
@@ -7479,30 +7641,34 @@
       <c r="E31" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="F31" s="51" t="s">
+      <c r="F31" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E31,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>CADOFE008</v>
+      </c>
+      <c r="G31" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G31" s="49">
+      <c r="H31" s="49">
         <v>14</v>
       </c>
-      <c r="H31" s="51" t="s">
+      <c r="I31" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="I31" s="51" t="str">
-        <f>VLOOKUP(H31,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J31" s="51" t="str">
+        <f>VLOOKUP(I31,'Base de Gerentes'!A:B,2,)</f>
         <v>Gabriel Gomes</v>
       </c>
-      <c r="J31" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K31" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L31" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L31" s="52">
+      <c r="M31" s="52">
         <v>433.72</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="49">
         <v>31</v>
       </c>
@@ -7518,30 +7684,34 @@
       <c r="E32" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="F32" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="49">
+      <c r="F32" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E32,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>AROSMA005</v>
+      </c>
+      <c r="G32" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="49">
         <v>11</v>
       </c>
-      <c r="H32" s="51" t="s">
+      <c r="I32" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="I32" s="51" t="str">
-        <f>VLOOKUP(H32,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J32" s="51" t="str">
+        <f>VLOOKUP(I32,'Base de Gerentes'!A:B,2,)</f>
         <v>Carmem Silva</v>
       </c>
-      <c r="J32" s="51" t="s">
+      <c r="K32" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="K32" s="51" t="s">
+      <c r="L32" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="L32" s="52">
+      <c r="M32" s="52">
         <v>186.45</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="49">
         <v>32</v>
       </c>
@@ -7557,30 +7727,34 @@
       <c r="E33" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="F33" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G33" s="49">
+      <c r="F33" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E33,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>ERTAMA0014</v>
+      </c>
+      <c r="G33" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="49">
         <v>13</v>
       </c>
-      <c r="H33" s="51" t="s">
+      <c r="I33" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="I33" s="51" t="str">
-        <f>VLOOKUP(H33,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J33" s="51" t="str">
+        <f>VLOOKUP(I33,'Base de Gerentes'!A:B,2,)</f>
         <v>Julia Ramos</v>
       </c>
-      <c r="J33" s="51" t="s">
+      <c r="K33" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="K33" s="51" t="s">
+      <c r="L33" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L33" s="52">
+      <c r="M33" s="52">
         <v>349.05</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="49">
         <v>33</v>
       </c>
@@ -7596,30 +7770,34 @@
       <c r="E34" s="51" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G34" s="49">
+      <c r="F34" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E34,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>ARRAMA006</v>
+      </c>
+      <c r="G34" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="49">
         <v>9</v>
       </c>
-      <c r="H34" s="51" t="s">
+      <c r="I34" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="I34" s="51" t="str">
-        <f>VLOOKUP(H34,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J34" s="51" t="str">
+        <f>VLOOKUP(I34,'Base de Gerentes'!A:B,2,)</f>
         <v>Roberto Lopes</v>
       </c>
-      <c r="J34" s="51" t="s">
-        <v>24</v>
-      </c>
       <c r="K34" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="L34" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L34" s="52">
+      <c r="M34" s="52">
         <v>152.54999999999998</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="49">
         <v>34</v>
       </c>
@@ -7635,31 +7813,35 @@
       <c r="E35" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="F35" s="51" t="s">
+      <c r="F35" s="51" t="str">
+        <f>_xlfn.XLOOKUP(E35,'Base de Vendedores'!B:B,'Base de Vendedores'!J:J,"Não identificado",0)</f>
+        <v>EMTAFE0013</v>
+      </c>
+      <c r="G35" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G35" s="49">
+      <c r="H35" s="49">
         <v>15</v>
       </c>
-      <c r="H35" s="51" t="s">
+      <c r="I35" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="I35" s="51" t="str">
-        <f>VLOOKUP(H35,'Base de Gerentes'!A:B,2,)</f>
+      <c r="J35" s="51" t="str">
+        <f>VLOOKUP(I35,'Base de Gerentes'!A:B,2,)</f>
         <v>Julia Ramos</v>
       </c>
-      <c r="J35" s="51" t="s">
+      <c r="K35" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="K35" s="51" t="s">
+      <c r="L35" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="L35" s="52">
+      <c r="M35" s="52">
         <v>975</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L35" xr:uid="{CFF5F63A-A48A-466D-9D12-E052B07C29AE}"/>
+  <autoFilter ref="A1:M35" xr:uid="{CFF5F63A-A48A-466D-9D12-E052B07C29AE}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -7681,9 +7863,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>105</v>
-      </c>
+      <c r="A1" s="27"/>
       <c r="B1" s="27" t="s">
         <v>4</v>
       </c>

</xml_diff>